<commit_message>
Updated documentation Added scenarios for sprint 3, update profile and view items tracked. Removed the update inventory item scenario, per Dr. Corley's comments.
</commit_message>
<xml_diff>
--- a/sprints/Sprint 3/Sprint3Backlog.xlsx
+++ b/sprints/Sprint 3/Sprint3Backlog.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467F9DD4-D7B2-418D-B4BE-75549BE4A9D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0046A5AB-8753-464E-AD22-0CF04CC8754E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1605" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2775" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated documentation updated the sprint backlog. Changed the add/remove inventory task to complete
</commit_message>
<xml_diff>
--- a/sprints/Sprint 3/Sprint3Backlog.xlsx
+++ b/sprints/Sprint 3/Sprint3Backlog.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0046A5AB-8753-464E-AD22-0CF04CC8754E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A495A2-B60C-4DB0-98D8-D1F884CEF181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="24765" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Progress</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Implement view for a member to view his profile </t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +442,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -459,7 +462,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -479,7 +482,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Updated Employee Wireframe and sprint backlog
</commit_message>
<xml_diff>
--- a/sprints/Sprint 3/Sprint3Backlog.xlsx
+++ b/sprints/Sprint 3/Sprint3Backlog.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A495A2-B60C-4DB0-98D8-D1F884CEF181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC0D27B-84B3-41CF-BB3C-29C4FFA27947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="24765" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Progress</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>DEADLINE</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Luke</t>
@@ -415,10 +412,15 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="65.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -442,16 +444,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>43885</v>
@@ -462,16 +464,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
         <v>43885</v>
@@ -482,16 +484,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
         <v>43885</v>
@@ -502,16 +504,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2">
         <v>43885</v>
@@ -522,16 +524,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2">
         <v>43885</v>
@@ -542,16 +544,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2">
         <v>43885</v>
@@ -562,16 +564,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="E8" s="2">
         <v>43885</v>

</xml_diff>